<commit_message>
Avance Carrito, Venta y Articulos
</commit_message>
<xml_diff>
--- a/Archivos de Datos/ListaArticulos.xlsx
+++ b/Archivos de Datos/ListaArticulos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -434,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -536,198 +536,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>24900</v>
-      </c>
-      <c r="F4">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4">
-        <v>112050</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>24900</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5">
-        <v>112050</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>24900</v>
-      </c>
-      <c r="F6">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6">
-        <v>112050</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>24900</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7">
-        <v>112050</v>
-      </c>
-      <c r="J7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>24900</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8">
-        <v>112050</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9">
-        <v>24900</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9">
-        <v>112050</v>
-      </c>
-      <c r="J9">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Avanzando en las funciones
</commit_message>
<xml_diff>
--- a/Archivos de Datos/ListaArticulos.xlsx
+++ b/Archivos de Datos/ListaArticulos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -434,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -536,198 +536,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>24900</v>
-      </c>
-      <c r="F4">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4">
-        <v>112050</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>24900</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5">
-        <v>112050</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>24900</v>
-      </c>
-      <c r="F6">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6">
-        <v>112050</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>24900</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7">
-        <v>112050</v>
-      </c>
-      <c r="J7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>24900</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8">
-        <v>112050</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9">
-        <v>24900</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9">
-        <v>112050</v>
-      </c>
-      <c r="J9">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>